<commit_message>
fix internal data and qc_test_climatology
</commit_message>
<xml_diff>
--- a/data-raw/qc_thresholds.xlsx
+++ b/data-raw/qc_thresholds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Dempsey\Desktop\RProjects\Packages\qaqcmar\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BBA26A-E6FB-46B6-8054-CC90699A190B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6731CF17-5930-405B-BCF3-4E52009DA211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4770" yWindow="150" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
   </bookViews>
@@ -100,7 +100,7 @@
     <t>vemco</t>
   </si>
   <si>
-    <t>month</t>
+    <t>numeric_month</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: add spike test
</commit_message>
<xml_diff>
--- a/data-raw/qc_thresholds.xlsx
+++ b/data-raw/qc_thresholds.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Dempsey\Desktop\RProjects\Packages\qaqcmar\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD59BF8-85E9-4279-8F56-A7A9F500D961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14869A7-FCA0-4EC4-A457-38B335C02944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
   </bookViews>
   <sheets>
     <sheet name="climatology" sheetId="1" r:id="rId1"/>
-    <sheet name="seasons" sheetId="3" r:id="rId2"/>
-    <sheet name="grossrange" sheetId="2" r:id="rId3"/>
+    <sheet name="grossrange" sheetId="2" r:id="rId2"/>
+    <sheet name="seasons" sheetId="3" r:id="rId3"/>
+    <sheet name="spike" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
   <si>
     <t>winter</t>
   </si>
@@ -107,6 +108,12 @@
   </si>
   <si>
     <t>vr2ar</t>
+  </si>
+  <si>
+    <t>threshold_high</t>
+  </si>
+  <si>
+    <t>threshold_low</t>
   </si>
 </sst>
 </file>
@@ -469,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3060FA24-756B-42C4-88A3-409ACE0ACD4A}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -729,132 +736,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBE0F9E-9FD4-4DDF-8390-3930E7ACA925}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AA8485-BA5D-4070-87F2-2B5EFA3D78A7}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,4 +940,212 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBE0F9E-9FD4-4DDF-8390-3930E7ACA925}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0881FE-BC0C-4A84-A701-CB88145A8D72}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
save thresholds internal dataset as long dataframe instead of list so will work with qaqcmar_thresholds dashboard
</commit_message>
<xml_diff>
--- a/data-raw/qc_thresholds.xlsx
+++ b/data-raw/qc_thresholds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Dempsey\Desktop\RProjects\Packages\qaqcmar\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14869A7-FCA0-4EC4-A457-38B335C02944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06927A06-9964-4C07-82F5-4D28722DEAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
+    <workbookView xWindow="2205" yWindow="0" windowWidth="24840" windowHeight="15600" activeTab="3" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
   </bookViews>
   <sheets>
     <sheet name="climatology" sheetId="1" r:id="rId1"/>
@@ -110,10 +110,10 @@
     <t>vr2ar</t>
   </si>
   <si>
-    <t>threshold_high</t>
-  </si>
-  <si>
-    <t>threshold_low</t>
+    <t>spike_high</t>
+  </si>
+  <si>
+    <t>spike_low</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B2" sqref="B2:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C2" sqref="C2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,7 +1068,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
works as expected with qaqcmar_thresholds
</commit_message>
<xml_diff>
--- a/data-raw/qc_thresholds.xlsx
+++ b/data-raw/qc_thresholds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Dempsey\Desktop\RProjects\Packages\qaqcmar\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06927A06-9964-4C07-82F5-4D28722DEAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2AF4A4-07EF-4DFC-AAA6-DEC4D8C16915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="0" windowWidth="24840" windowHeight="15600" activeTab="3" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
   </bookViews>
   <sheets>
     <sheet name="climatology" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>salinity_psu</t>
   </si>
   <si>
-    <t>temperature_degree_C</t>
-  </si>
-  <si>
     <t>spring</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>sensor_type</t>
   </si>
   <si>
-    <t>dissolved_oxygen_uncorrected_mg_per_L</t>
-  </si>
-  <si>
     <t>vr2ar</t>
   </si>
   <si>
@@ -114,6 +108,12 @@
   </si>
   <si>
     <t>spike_low</t>
+  </si>
+  <si>
+    <t>dissolved_oxygen_uncorrected_mg_per_l</t>
+  </si>
+  <si>
+    <t>temperature_degree_c</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B17"/>
+      <selection activeCell="A14" sqref="A14:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,21 +490,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -532,10 +532,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>70</v>
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>70</v>
@@ -605,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>70</v>
@@ -633,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -647,7 +647,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -661,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -686,10 +686,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
         <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -700,10 +700,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>7</v>
@@ -714,10 +714,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -740,7 +740,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,30 +755,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -818,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -835,10 +835,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -855,10 +855,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -875,10 +875,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>-5</v>
@@ -895,10 +895,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>-40</v>
@@ -915,10 +915,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>-5</v>
@@ -954,10 +954,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -990,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1068,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,18 +1080,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>2</v>

</xml_diff>

<commit_message>
remove NA column that was the result of not including sensor_depth_measured_m in the climatology_table
</commit_message>
<xml_diff>
--- a/data-raw/qc_thresholds.xlsx
+++ b/data-raw/qc_thresholds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Dempsey\Desktop\RProjects\Packages\qaqcmar\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2AF4A4-07EF-4DFC-AAA6-DEC4D8C16915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4577656-A78B-4910-A774-A894A906D8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F929B56-69A8-4A8B-9107-39E6EC01019B}"/>
   </bookViews>
   <sheets>
     <sheet name="climatology" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="26">
   <si>
     <t>winter</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>temperature_degree_c</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3060FA24-756B-42C4-88A3-409ACE0ACD4A}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,6 +727,62 @@
       </c>
       <c r="D17">
         <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1067,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0881FE-BC0C-4A84-A701-CB88145A8D72}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>